<commit_message>
SE_3.py done and begining to finish the interface
</commit_message>
<xml_diff>
--- a/SE/trabalhofinal.xlsx
+++ b/SE/trabalhofinal.xlsx
@@ -1074,7 +1074,7 @@
         <v>13.33410601384405</v>
       </c>
       <c r="C64">
-        <v>9.600556329967716</v>
+        <v>9.600556329967715</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1272,7 +1272,7 @@
         <v>11.71517058833568</v>
       </c>
       <c r="C82">
-        <v>8.434922823601692</v>
+        <v>8.43492282360169</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1995,7 +1995,7 @@
         <v>2</v>
       </c>
       <c r="B148">
-        <v>0.08518085051142056</v>
+        <v>0.08518085051142057</v>
       </c>
       <c r="C148">
         <v>0.153325530920557</v>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="B188">
-        <v>2.911712792871184</v>
+        <v>2.911712792871185</v>
       </c>
       <c r="C188">
         <v>2.096433210867253</v>
@@ -2449,7 +2449,7 @@
         <v>29.14422386966211</v>
       </c>
       <c r="C189">
-        <v>0.1199076639208955</v>
+        <v>0.1199076639208956</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -2490,10 +2490,10 @@
         <v>2</v>
       </c>
       <c r="B193">
-        <v>0.08517991333332568</v>
+        <v>0.08517991333332571</v>
       </c>
       <c r="C193">
-        <v>0.1533238439999862</v>
+        <v>0.1533238439999863</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3579,10 +3579,10 @@
         <v>5</v>
       </c>
       <c r="B292">
-        <v>5.400951173490634</v>
+        <v>5.400951173490633</v>
       </c>
       <c r="C292">
-        <v>3.888684844913257</v>
+        <v>3.888684844913256</v>
       </c>
     </row>
     <row r="293" spans="1:3">
@@ -3788,10 +3788,10 @@
         <v>5</v>
       </c>
       <c r="B311">
-        <v>0.4258977431721957</v>
+        <v>0.4258977431721958</v>
       </c>
       <c r="C311">
-        <v>0.3066463750839809</v>
+        <v>0.306646375083981</v>
       </c>
     </row>
     <row r="312" spans="1:3">
@@ -5529,7 +5529,7 @@
         <v>1.218102768154924</v>
       </c>
       <c r="C469">
-        <v>0.8770339930715451</v>
+        <v>0.8770339930715453</v>
       </c>
     </row>
     <row r="470" spans="1:3">
@@ -6783,7 +6783,7 @@
         <v>0.1400711681721312</v>
       </c>
       <c r="C583">
-        <v>0.1008512410839344</v>
+        <v>0.1008512410839345</v>
       </c>
     </row>
     <row r="584" spans="1:3">
@@ -7487,7 +7487,7 @@
         <v>1.081976746732375</v>
       </c>
       <c r="C647">
-        <v>0.7790232576473097</v>
+        <v>0.77902325764731</v>
       </c>
     </row>
     <row r="648" spans="1:3">
@@ -8158,7 +8158,7 @@
         <v>1.150234852493529</v>
       </c>
       <c r="C708">
-        <v>0.8281690937953412</v>
+        <v>0.828169093795341</v>
       </c>
     </row>
     <row r="709" spans="1:3">
@@ -8540,7 +8540,7 @@
         <v>5</v>
       </c>
       <c r="B743">
-        <v>1.750534708013383</v>
+        <v>1.750534708013384</v>
       </c>
       <c r="C743">
         <v>1.260384989769636</v>
@@ -8551,10 +8551,10 @@
         <v>5</v>
       </c>
       <c r="B744">
-        <v>0.798221332768946</v>
+        <v>0.7982213327689459</v>
       </c>
       <c r="C744">
-        <v>0.5747193595936412</v>
+        <v>0.5747193595936411</v>
       </c>
     </row>
     <row r="745" spans="1:3">
@@ -8851,7 +8851,7 @@
         <v>1.164918085977198</v>
       </c>
       <c r="C771">
-        <v>0.8387410219035826</v>
+        <v>0.8387410219035824</v>
       </c>
     </row>
     <row r="772" spans="1:3">
@@ -10102,10 +10102,10 @@
         <v>5</v>
       </c>
       <c r="B885">
-        <v>0.8872659473739439</v>
+        <v>0.8872659473739437</v>
       </c>
       <c r="C885">
-        <v>0.6388314821092396</v>
+        <v>0.6388314821092395</v>
       </c>
     </row>
     <row r="886" spans="1:3">
@@ -10894,10 +10894,10 @@
         <v>5</v>
       </c>
       <c r="B957">
-        <v>0.9369745551292104</v>
+        <v>0.9369745551292106</v>
       </c>
       <c r="C957">
-        <v>0.6746216796930314</v>
+        <v>0.6746216796930316</v>
       </c>
     </row>
     <row r="958" spans="1:3">
@@ -11433,10 +11433,10 @@
         <v>5</v>
       </c>
       <c r="B1006">
-        <v>3.253969388713834</v>
+        <v>3.253969388713835</v>
       </c>
       <c r="C1006">
-        <v>2.34285795987396</v>
+        <v>2.342857959873961</v>
       </c>
     </row>
     <row r="1007" spans="1:3">
@@ -12272,7 +12272,7 @@
         <v>2.615163333978041</v>
       </c>
       <c r="C1082">
-        <v>1.88291760046419</v>
+        <v>1.882917600464189</v>
       </c>
     </row>
     <row r="1083" spans="1:3">
@@ -12393,7 +12393,7 @@
         <v>0.406873473107109</v>
       </c>
       <c r="C1093">
-        <v>0.7323722515927963</v>
+        <v>0.7323722515927962</v>
       </c>
     </row>
     <row r="1094" spans="1:3">
@@ -14975,7 +14975,7 @@
         <v>5</v>
       </c>
       <c r="B1328">
-        <v>7.267586131036627</v>
+        <v>7.267586131036628</v>
       </c>
       <c r="C1328">
         <v>5.232662014346372</v>
@@ -15286,7 +15286,7 @@
         <v>0.2034371522691132</v>
       </c>
       <c r="C1356">
-        <v>0.3661868740844037</v>
+        <v>0.3661868740844038</v>
       </c>
     </row>
     <row r="1357" spans="1:3">
@@ -15811,7 +15811,7 @@
         <v>5</v>
       </c>
       <c r="B1404">
-        <v>0.8192390826092124</v>
+        <v>0.8192390826092125</v>
       </c>
       <c r="C1404">
         <v>0.589852139478633</v>
@@ -16185,7 +16185,7 @@
         <v>4395</v>
       </c>
       <c r="B1438">
-        <v>26.86464816920173</v>
+        <v>26.86464816920172</v>
       </c>
       <c r="C1438">
         <v>0.02200517256180346</v>
@@ -16251,10 +16251,10 @@
         <v>2</v>
       </c>
       <c r="B1444">
-        <v>0.5409893137210028</v>
+        <v>0.5409893137210029</v>
       </c>
       <c r="C1444">
-        <v>0.9737807646978051</v>
+        <v>0.9737807646978053</v>
       </c>
     </row>
     <row r="1445" spans="1:3">
@@ -16328,10 +16328,10 @@
         <v>5</v>
       </c>
       <c r="B1451">
-        <v>8.061542879077336</v>
+        <v>8.061542879077335</v>
       </c>
       <c r="C1451">
-        <v>5.804310872935683</v>
+        <v>5.804310872935681</v>
       </c>
     </row>
     <row r="1452" spans="1:3">
@@ -16966,7 +16966,7 @@
         <v>2</v>
       </c>
       <c r="B1509">
-        <v>0.2034374573067695</v>
+        <v>0.2034374573067696</v>
       </c>
       <c r="C1509">
         <v>0.3661874231521852</v>
@@ -17739,7 +17739,7 @@
         <v>1.295173945647843</v>
       </c>
       <c r="C1579">
-        <v>0.9325252408664471</v>
+        <v>0.9325252408664473</v>
       </c>
     </row>
     <row r="1580" spans="1:3">
@@ -17890,10 +17890,10 @@
         <v>5</v>
       </c>
       <c r="B1593">
-        <v>4.27781669252769</v>
+        <v>4.277816692527689</v>
       </c>
       <c r="C1593">
-        <v>3.080028018619937</v>
+        <v>3.080028018619936</v>
       </c>
     </row>
     <row r="1594" spans="1:3">
@@ -17904,7 +17904,7 @@
         <v>3.72634382103098</v>
       </c>
       <c r="C1594">
-        <v>2.682967551142306</v>
+        <v>2.682967551142305</v>
       </c>
     </row>
     <row r="1595" spans="1:3">
@@ -17956,10 +17956,10 @@
         <v>2</v>
       </c>
       <c r="B1599">
-        <v>0.3745681737552018</v>
+        <v>0.3745681737552017</v>
       </c>
       <c r="C1599">
-        <v>0.6742227127593633</v>
+        <v>0.6742227127593632</v>
       </c>
     </row>
     <row r="1600" spans="1:3">
@@ -18132,7 +18132,7 @@
         <v>5</v>
       </c>
       <c r="B1615">
-        <v>5.583358956827385</v>
+        <v>5.583358956827386</v>
       </c>
       <c r="C1615">
         <v>4.020018448915717</v>
@@ -18913,10 +18913,10 @@
         <v>5</v>
       </c>
       <c r="B1686">
-        <v>6.564340382850035</v>
+        <v>6.564340382850033</v>
       </c>
       <c r="C1686">
-        <v>4.726325075652025</v>
+        <v>4.726325075652024</v>
       </c>
     </row>
     <row r="1687" spans="1:3">

</xml_diff>